<commit_message>
Excel expanded and visuals updated
</commit_message>
<xml_diff>
--- a/data/Vulplanning.xlsx
+++ b/data/Vulplanning.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="71">
   <si>
     <t/>
   </si>
@@ -23,64 +23,205 @@
     <t>Vultijd:</t>
   </si>
   <si>
+    <t>797.54579041648</t>
+  </si>
+  <si>
+    <t>Vracht:</t>
+  </si>
+  <si>
+    <t>785</t>
+  </si>
+  <si>
+    <t>Ploeg:</t>
+  </si>
+  <si>
+    <t>Paden</t>
+  </si>
+  <si>
+    <t>Vracht</t>
+  </si>
+  <si>
+    <t>Vultijd</t>
+  </si>
+  <si>
+    <t>Taken</t>
+  </si>
+  <si>
+    <t>Gijs Vermeul</t>
+  </si>
+  <si>
+    <t>Internationaal</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Spiegelen Internationaal</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>Eric Bull</t>
+  </si>
+  <si>
+    <t>Potjes</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
     <t>0</t>
   </si>
   <si>
-    <t>Vracht:</t>
-  </si>
-  <si>
-    <t>Ploeg:</t>
-  </si>
-  <si>
-    <t>Paden</t>
-  </si>
-  <si>
-    <t>Vracht</t>
-  </si>
-  <si>
-    <t>Vultijd</t>
-  </si>
-  <si>
-    <t>Eric Bull</t>
-  </si>
-  <si>
-    <t>Internationaal</t>
+    <t>Spiegelen Potjes</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>Minte Eskes</t>
+  </si>
+  <si>
+    <t>Frisdrank</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>Spiegelen Frisdrank</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Pien Zwinkels</t>
+  </si>
+  <si>
+    <t>Bier</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>Spiegelen Bier</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Burton Braam</t>
+  </si>
+  <si>
+    <t>Wijn</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Spiegelen Chips</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Wessel Horsthuis</t>
+  </si>
+  <si>
+    <t>Chips</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Spiegelen Wijn</t>
+  </si>
+  <si>
+    <t>Niels Koppe</t>
+  </si>
+  <si>
+    <t>Cosmetica</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>Spiegelen Dierenvoeding</t>
+  </si>
+  <si>
+    <t>Wouter Swijnenburg</t>
+  </si>
+  <si>
+    <t>Dierenvoeding</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>Spiegelen Cosmetica</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Gijs Vellekoop</t>
+  </si>
+  <si>
+    <t>Koek</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>Spiegelen Koek</t>
+  </si>
+  <si>
+    <t>Jasper Beukel</t>
+  </si>
+  <si>
+    <t>Ontbijt</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>Spiegelen Ontbijt</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>Esmée de Waal</t>
+  </si>
+  <si>
+    <t>Zuivel</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Spiegelen Zuivel</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Lucas Clavel</t>
+  </si>
+  <si>
+    <t>VVP</t>
+  </si>
+  <si>
+    <t>Spiegelen VVP</t>
   </si>
   <si>
     <t>-1</t>
-  </si>
-  <si>
-    <t>Potjes</t>
-  </si>
-  <si>
-    <t>Frisdrank</t>
-  </si>
-  <si>
-    <t>Bier</t>
-  </si>
-  <si>
-    <t>Wijn</t>
-  </si>
-  <si>
-    <t>Chips</t>
-  </si>
-  <si>
-    <t>Cosmetica</t>
-  </si>
-  <si>
-    <t>Dierenvoeding</t>
-  </si>
-  <si>
-    <t>Koek</t>
-  </si>
-  <si>
-    <t>Ontbijt</t>
-  </si>
-  <si>
-    <t>Zuivel</t>
-  </si>
-  <si>
-    <t>VVP</t>
   </si>
   <si>
     <t>Diepvries</t>
@@ -128,7 +269,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -152,7 +293,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -160,16 +301,19 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -177,13 +321,24 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5"/>
@@ -192,13 +347,24 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7"/>
@@ -207,13 +373,24 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9"/>
@@ -222,13 +399,24 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
-        <v>3</v>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11"/>
@@ -237,13 +425,24 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="13"/>
@@ -252,13 +451,24 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="15"/>
@@ -267,13 +477,24 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17"/>
@@ -282,13 +503,24 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>48</v>
+      </c>
+      <c r="E18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="19"/>
@@ -297,13 +529,24 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="21"/>
@@ -312,13 +555,24 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>57</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="23"/>
@@ -327,13 +581,24 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>21</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>3</v>
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="25"/>
@@ -342,13 +607,24 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>40</v>
+      </c>
+      <c r="E26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27"/>
@@ -357,13 +633,24 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>20</v>
+      </c>
+      <c r="E28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="29"/>

</xml_diff>